<commit_message>
Ensure all forms are up to date
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/enrollment/enrollment.xlsx
+++ b/app/config/tables/business/forms/enrollment/enrollment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="760" windowWidth="34520" windowHeight="20040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1400" yWindow="1900" windowWidth="34520" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="323">
   <si>
     <t>comments</t>
   </si>
@@ -1010,6 +1010,12 @@
 subsector.display = {title: {text:{default:subsector.subsector_txt, sw:subsector.subsector_txt_sw }}};
 return subsector;
 })</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>(data('enrollment_date') !== null &amp;&amp; data('enrollment_date') !== undefined) ? data('enrollment_date') : new Date()</t>
   </si>
 </sst>
 </file>
@@ -1965,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2081,10 +2087,18 @@
       <c r="H3" s="6"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="120">
       <c r="A4" s="24"/>
+      <c r="D4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="H4" s="6"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="2" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="30" t="s">
@@ -2673,7 +2687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3734,7 +3748,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Add region and second primary phone number field for validation, fix strings
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/enrollment/enrollment.xlsx
+++ b/app/config/tables/business/forms/enrollment/enrollment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5120" yWindow="6080" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="332">
   <si>
     <t>comments</t>
   </si>
@@ -696,9 +696,6 @@
     <t>constraint</t>
   </si>
   <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
     <t>select_one_with_other</t>
   </si>
   <si>
@@ -795,18 +792,9 @@
     <t>decline_business_owner_age</t>
   </si>
   <si>
-    <t>Business owner age must be between 15 and 100</t>
-  </si>
-  <si>
-    <t>constraint_message.sw</t>
-  </si>
-  <si>
     <t>sw:Business owner age must be between 15 and 100</t>
   </si>
   <si>
-    <t>Size of the firm must be greater than 0</t>
-  </si>
-  <si>
     <t>sw:Size of the firm must be greater than 0</t>
   </si>
   <si>
@@ -871,18 +859,6 @@
   </si>
   <si>
     <t>phone_number_validation</t>
-  </si>
-  <si>
-    <t>(function(){
-  var phNum = data('phone_number');
-  if (phNum === null || phNum === undefined) {
-    return false;
-  } else {
-    if (phNum.length &lt; 10) { return false;}
-    if (phNum.charAt(0) !== '0') { return false; }
-    return true;
-  }
-})()</t>
   </si>
   <si>
     <t>secondary_phone_number_validation</t>
@@ -1004,6 +980,80 @@
   </si>
   <si>
     <t>(data('enrollment_date') !== null &amp;&amp; data('enrollment_date') !== undefined) ? data('enrollment_date') : new Date()</t>
+  </si>
+  <si>
+    <t>region_group_by</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Choose the region.</t>
+  </si>
+  <si>
+    <t>sw:Choose the region.</t>
+  </si>
+  <si>
+    <t>region=?</t>
+  </si>
+  <si>
+    <t>[data('region')]</t>
+  </si>
+  <si>
+    <t>primary_phone_number</t>
+  </si>
+  <si>
+    <t>primary_phone_number_validation</t>
+  </si>
+  <si>
+    <t>(function(){
+  var phNum = data('primary_phone_number');
+  if (phNum === null || phNum === undefined) {
+    return false;
+  } else {
+    if (phNum.length &lt; 10) { return false;}
+    if (phNum.charAt(0) !== '0') { return false; }
+    return true;
+  }
+})()</t>
+  </si>
+  <si>
+    <t>(data('consent') !== 'yes') || calculates.primary_phone_number_validation()</t>
+  </si>
+  <si>
+    <t>(function(){
+  var phNum = data('phone_number');
+  if (phNum === null || phNum === undefined) {
+    return false;
+  } else {
+    var primaryPhNum = data('primary_phone_number');
+    if (phNum !== primaryPhNum) { return false; }
+    if (phNum.length &lt; 10) { return false;}
+    if (phNum.charAt(0) !== '0') { return false; }
+    return true;
+  }
+})()</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.sw</t>
+  </si>
+  <si>
+    <t>Business owner age must be between 15 and 100.</t>
+  </si>
+  <si>
+    <t>Size of the firm must be greater than 0.</t>
+  </si>
+  <si>
+    <t>Phone number must begin with 0 and be 10 digits.</t>
+  </si>
+  <si>
+    <t>sw:Phone number must begin with 0 and be 10 digits.</t>
+  </si>
+  <si>
+    <t>Phone number must begin with 0, be 10 digits, and match previously entered phone number.</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1124,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1111,12 +1161,6 @@
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1127,7 +1171,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="174">
+  <cellStyleXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1230,6 +1274,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1367,9 +1445,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1377,8 +1452,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="174">
+  <cellStyles count="208">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1465,6 +1543,23 @@
     <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1550,6 +1645,23 @@
     <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Normal 5" xfId="101"/>
@@ -1957,10 +2069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1984,7 +2096,7 @@
     <col min="1026" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="24">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2031,13 +2143,13 @@
         <v>222</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>223</v>
+        <v>325</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>257</v>
+        <v>326</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -2070,7 +2182,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H3" s="6"/>
       <c r="M3" s="2"/>
@@ -2078,585 +2190,649 @@
     <row r="4" spans="1:18" ht="120">
       <c r="A4" s="24"/>
       <c r="D4" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="H4" s="6"/>
       <c r="M4" s="2" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="30" t="s">
+      <c r="N6" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H7" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="30" t="s">
+      <c r="N7" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="30" t="s">
+      <c r="N8" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H9" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="30" t="s">
+      <c r="N9" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="60">
+      <c r="A10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="60">
-      <c r="A10" s="30" t="s">
+      <c r="N11" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="60">
+      <c r="A12" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D12" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H12" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="L10" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-    </row>
-    <row r="11" spans="1:18" s="9" customFormat="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-    </row>
-    <row r="12" spans="1:18" s="9" customFormat="1" ht="216">
-      <c r="A12" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="N12" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="P12" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q12" s="28" t="s">
-        <v>266</v>
-      </c>
+      <c r="L12" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
     </row>
     <row r="13" spans="1:18" s="9" customFormat="1">
-      <c r="A13" s="30"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="9" t="s">
         <v>103</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="H13" s="7"/>
+        <v>295</v>
+      </c>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
-      <c r="Q13" s="28"/>
-    </row>
-    <row r="14" spans="1:18" s="9" customFormat="1" ht="84">
-      <c r="A14" s="30"/>
+      <c r="Q13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" s="9" customFormat="1" ht="216">
+      <c r="A14" s="29" t="s">
+        <v>201</v>
+      </c>
       <c r="D14" s="9" t="s">
-        <v>23</v>
+        <v>257</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="N14" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="P14" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q14" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="G14" s="9" t="s">
+    </row>
+    <row r="15" spans="1:18" s="9" customFormat="1">
+      <c r="A15" s="29"/>
+      <c r="B15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="N14" s="25" t="s">
-        <v>280</v>
-      </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-    </row>
-    <row r="15" spans="1:18" s="9" customFormat="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="9" t="s">
-        <v>173</v>
-      </c>
+      <c r="H15" s="7"/>
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-    </row>
-    <row r="16" spans="1:18" s="9" customFormat="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="N16" s="25"/>
+      <c r="Q15" s="28"/>
+    </row>
+    <row r="16" spans="1:18" s="9" customFormat="1" ht="84">
+      <c r="A16" s="29"/>
+      <c r="D16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>276</v>
+      </c>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
       <c r="Q16" s="25"/>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:18" s="9" customFormat="1">
+      <c r="A17" s="29"/>
+      <c r="B17" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="1:18" s="9" customFormat="1">
+      <c r="A18" s="29"/>
+      <c r="B18" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H19" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="30"/>
-      <c r="B18" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:18" ht="101" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="N19" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="29"/>
+      <c r="B20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:18" ht="101" customHeight="1">
+      <c r="A21" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="P19" s="2" t="s">
+      <c r="N21" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q21" s="26" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="84">
+      <c r="A22" s="29"/>
+      <c r="D22" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="29"/>
+      <c r="B23" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:18" ht="24">
+      <c r="A24" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="48">
+      <c r="A25" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="N25" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q25" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="Q19" s="26" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="84">
-      <c r="A20" s="30"/>
-      <c r="D20" s="1" t="s">
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="29"/>
+      <c r="B26" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="N26" s="23"/>
+      <c r="Q26" s="26"/>
+    </row>
+    <row r="27" spans="1:18" s="10" customFormat="1" ht="60">
+      <c r="A27" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="N27" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="30"/>
-      <c r="B21" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:18" ht="24">
-      <c r="A22" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="48">
-      <c r="A23" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="N23" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q23" s="26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="30"/>
-      <c r="B24" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="12"/>
-      <c r="N24" s="23"/>
-      <c r="Q24" s="26"/>
-    </row>
-    <row r="25" spans="1:18" s="10" customFormat="1" ht="48">
-      <c r="A25" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="N25" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="O25" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="30" t="s">
+      <c r="O27" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="P27" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q27" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="N26" s="23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="30"/>
-      <c r="B27" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H27" s="6"/>
-      <c r="N27" s="23"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="30"/>
-      <c r="B28" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H28" s="6"/>
-      <c r="N28" s="23"/>
+      <c r="N28" s="23" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="30"/>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="N29" s="23" t="s">
-        <v>247</v>
-      </c>
+      <c r="A29" s="29"/>
+      <c r="B29" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="N29" s="23"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>306</v>
+        <v>267</v>
       </c>
       <c r="H30" s="6"/>
       <c r="N30" s="23"/>
     </row>
-    <row r="31" spans="1:18" s="10" customFormat="1" ht="96">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:18">
+      <c r="A31" s="29"/>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="N31" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="29"/>
+      <c r="B32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" spans="1:18" s="10" customFormat="1" ht="96">
+      <c r="A33" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H33" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="N31" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="O31" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="48">
-      <c r="A32" s="30" t="s">
+      <c r="N33" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="P33" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q33" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="48">
+      <c r="A34" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H34" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="N32" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="30"/>
-      <c r="B33" s="1" t="s">
+      <c r="N34" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="29"/>
+      <c r="B35" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="30"/>
-      <c r="B34" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="30"/>
-      <c r="B35" s="1" t="s">
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="29"/>
+      <c r="B36" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="29"/>
+      <c r="B37" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="29"/>
+      <c r="D38" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="30"/>
-      <c r="D36" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="30"/>
-      <c r="B37" s="1" t="s">
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="29"/>
+      <c r="B39" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2673,10 +2849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2731,7 +2907,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>314</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>91</v>
@@ -2755,12 +2931,12 @@
         <v>95</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>241</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>91</v>
@@ -2772,10 +2948,10 @@
         <v>92</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>96</v>
+        <v>318</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>99</v>
+        <v>319</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>95</v>
@@ -2784,12 +2960,12 @@
         <v>95</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="16" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>91</v>
@@ -2801,10 +2977,10 @@
         <v>92</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>244</v>
+        <v>96</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>245</v>
+        <v>99</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>95</v>
@@ -2813,26 +2989,55 @@
         <v>95</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1">
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="7" spans="1:11" ht="85" customHeight="1">
-      <c r="A7" s="8" t="s">
+    <row r="6" spans="1:11" ht="16" customHeight="1">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="85" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>316</v>
+      <c r="D8" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +3088,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>106</v>
@@ -2897,7 +3102,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>58</v>
@@ -2911,7 +3116,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>59</v>
@@ -2925,7 +3130,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>60</v>
@@ -2939,7 +3144,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>111</v>
@@ -2953,7 +3158,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>113</v>
@@ -2967,7 +3172,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>115</v>
@@ -2981,7 +3186,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>61</v>
@@ -3034,7 +3239,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>62</v>
@@ -3048,7 +3253,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>63</v>
@@ -3062,16 +3267,16 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3085,7 +3290,7 @@
         <v>194</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3099,7 +3304,7 @@
         <v>197</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3191,7 +3396,7 @@
         <v>118</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>123</v>
@@ -3205,7 +3410,7 @@
         <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>125</v>
@@ -3219,7 +3424,7 @@
         <v>118</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>127</v>
@@ -3331,7 +3536,7 @@
         <v>118</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>143</v>
@@ -3513,7 +3718,7 @@
         <v>118</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>169</v>
@@ -3527,69 +3732,69 @@
         <v>118</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B59" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C59" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B60" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C60" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D60" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
+        <v>286</v>
+      </c>
+      <c r="B61" t="s">
         <v>291</v>
       </c>
-      <c r="B61" t="s">
-        <v>296</v>
-      </c>
       <c r="C61" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D61" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B62" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C62" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D62" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3608,7 +3813,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3720,10 +3925,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3753,12 +3958,12 @@
       <c r="B2" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
         <v>80</v>
@@ -3767,7 +3972,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
         <v>71</v>
@@ -3776,7 +3981,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -3807,7 +4012,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -3818,7 +4023,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
         <v>101</v>
@@ -3830,7 +4035,7 @@
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1">
       <c r="A10" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>104</v>
@@ -3843,7 +4048,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="14" customFormat="1">
@@ -3868,10 +4073,10 @@
     </row>
     <row r="14" spans="1:8" s="14" customFormat="1">
       <c r="A14" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="14" customFormat="1">
@@ -3906,7 +4111,7 @@
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1">
       <c r="A18" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>73</v>
@@ -3919,7 +4124,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="14" customFormat="1">
@@ -3934,7 +4139,7 @@
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1">
       <c r="A21" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>74</v>
@@ -3963,7 +4168,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3992,33 +4197,41 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4058,7 +4271,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="21" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>83</v>
@@ -4082,37 +4295,45 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="211" customHeight="1">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="174" customHeight="1">
+      <c r="A3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="144">
-      <c r="A2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="156">
-      <c r="A3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>284</v>
+    </row>
+    <row r="4" spans="1:2" ht="175" customHeight="1">
+      <c r="A4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>

<commit_message>
Add new option and question to enrollment form
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/enrollment/enrollment.xlsx
+++ b/app/config/tables/business/forms/enrollment/enrollment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2780" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="346">
   <si>
     <t>comments</t>
   </si>
@@ -1081,6 +1081,21 @@
   </si>
   <si>
     <t>sw:Do you specialize in a specifc crop or livestock?</t>
+  </si>
+  <si>
+    <t>Enter the subvillage</t>
+  </si>
+  <si>
+    <t>sw:Enter the subvilllage</t>
+  </si>
+  <si>
+    <t>not_applicable</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>sw:Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="242">
+  <cellStyleXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1311,6 +1326,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1540,7 +1557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="242">
+  <cellStyles count="244">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1661,6 +1678,7 @@
     <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1780,6 +1798,7 @@
     <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Normal 5" xfId="101"/>
@@ -2187,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2415,23 +2434,20 @@
       <c r="A9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="60">
+        <v>341</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="29" t="s">
         <v>12</v>
       </c>
@@ -2439,168 +2455,178 @@
         <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>148</v>
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="O10" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q10" s="26" t="s">
-        <v>266</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+    </row>
+    <row r="11" spans="1:18" ht="60">
       <c r="A11" s="29" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>141</v>
+        <v>256</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>148</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="60">
+      <c r="O11" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="29" t="s">
         <v>162</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="60">
+      <c r="A13" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G13" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H13" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L13" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N13" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-    </row>
-    <row r="13" spans="1:18" s="9" customFormat="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="9" t="s">
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+    </row>
+    <row r="14" spans="1:18" s="9" customFormat="1">
+      <c r="A14" s="29"/>
+      <c r="B14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-    </row>
-    <row r="14" spans="1:18" s="9" customFormat="1" ht="216">
-      <c r="A14" s="29" t="s">
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+    </row>
+    <row r="15" spans="1:18" s="9" customFormat="1" ht="216">
+      <c r="A15" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="N14" s="25" t="s">
+      <c r="N15" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="O14" s="25" t="s">
+      <c r="O15" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="P14" s="25" t="s">
+      <c r="P15" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="Q14" s="28" t="s">
+      <c r="Q15" s="28" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="9" customFormat="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="9" t="s">
+    <row r="16" spans="1:18" s="9" customFormat="1">
+      <c r="A16" s="29"/>
+      <c r="B16" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="28"/>
-    </row>
-    <row r="16" spans="1:18" s="9" customFormat="1" ht="84">
-      <c r="A16" s="29"/>
-      <c r="D16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="N16" s="25" t="s">
-        <v>223</v>
-      </c>
+      <c r="H16" s="7"/>
+      <c r="N16" s="25"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-    </row>
-    <row r="17" spans="1:18" s="9" customFormat="1">
+      <c r="Q16" s="28"/>
+    </row>
+    <row r="17" spans="1:18" s="9" customFormat="1" ht="84">
       <c r="A17" s="29"/>
-      <c r="B17" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="N17" s="25"/>
+      <c r="D17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>223</v>
+      </c>
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
@@ -2615,368 +2641,378 @@
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="13">
-      <c r="A19" s="33" t="s">
+    <row r="19" spans="1:18" s="9" customFormat="1">
+      <c r="A19" s="29"/>
+      <c r="B19" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+    </row>
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="13">
+      <c r="A20" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F20" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G20" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H20" s="35" t="s">
         <v>317</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H20" s="38" t="s">
-        <v>333</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>196</v>
       </c>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="29"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="29"/>
+      <c r="B22" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="1:18" ht="101" customHeight="1">
-      <c r="A22" s="29" t="s">
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:18" ht="101" customHeight="1">
+      <c r="A23" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O23" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="Q22" s="26" t="s">
+      <c r="Q23" s="26" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="84">
-      <c r="A23" s="29"/>
-      <c r="D23" s="1" t="s">
+    <row r="24" spans="1:18" ht="84">
+      <c r="A24" s="29"/>
+      <c r="D24" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H24" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="29"/>
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:18">
+      <c r="A25" s="29"/>
+      <c r="B25" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:18" ht="24">
-      <c r="A25" s="29" t="s">
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:18" ht="24">
+      <c r="A26" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H26" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="48">
-      <c r="A26" s="29" t="s">
+    <row r="27" spans="1:18" ht="48">
+      <c r="A27" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="H27" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N27" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="Q26" s="26" t="s">
+      <c r="Q27" s="26" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="29"/>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:18">
+      <c r="A28" s="29"/>
+      <c r="B28" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12"/>
-      <c r="N27" s="23"/>
-      <c r="Q27" s="26"/>
-    </row>
-    <row r="28" spans="1:18" s="10" customFormat="1" ht="60">
-      <c r="A28" s="29" t="s">
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
+      <c r="N28" s="23"/>
+      <c r="Q28" s="26"/>
+    </row>
+    <row r="29" spans="1:18" s="10" customFormat="1" ht="60">
+      <c r="A29" s="29" t="s">
         <v>217</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H29" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="N28" s="27" t="s">
+      <c r="N29" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="O28" s="27" t="s">
+      <c r="O29" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="P28" s="27" t="s">
+      <c r="P29" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="Q28" s="39" t="s">
+      <c r="Q29" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="R28" s="10" t="s">
+      <c r="R29" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="29" t="s">
+    <row r="30" spans="1:18">
+      <c r="A30" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H30" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="N29" s="23" t="s">
+      <c r="N30" s="23" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="29"/>
-      <c r="B30" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H30" s="6"/>
-      <c r="N30" s="23"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="29"/>
       <c r="B31" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H31" s="6"/>
       <c r="N31" s="23"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="29"/>
-      <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="N32" s="23" t="s">
-        <v>196</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="29"/>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="29"/>
+      <c r="B34" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H33" s="6"/>
-      <c r="N33" s="23"/>
-    </row>
-    <row r="34" spans="1:18" s="10" customFormat="1" ht="96">
-      <c r="A34" s="29" t="s">
+      <c r="H34" s="6"/>
+      <c r="N34" s="23"/>
+    </row>
+    <row r="35" spans="1:18" s="10" customFormat="1" ht="96">
+      <c r="A35" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H35" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="N34" s="27" t="s">
+      <c r="N35" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="O34" s="27" t="s">
+      <c r="O35" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="P34" s="27" t="s">
+      <c r="P35" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="Q34" s="39" t="s">
+      <c r="Q35" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="R34" s="10" t="s">
+      <c r="R35" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="48">
-      <c r="A35" s="29" t="s">
+    <row r="36" spans="1:18" ht="48">
+      <c r="A36" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H36" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="29"/>
-      <c r="B36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="29"/>
       <c r="B37" s="1" t="s">
-        <v>215</v>
+        <v>136</v>
       </c>
       <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="29"/>
       <c r="B38" s="1" t="s">
-        <v>197</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="29"/>
-      <c r="D39" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>336</v>
+      <c r="B39" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="29"/>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="29"/>
+      <c r="B41" s="1" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3199,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3855,6 +3891,20 @@
       </c>
       <c r="D52" t="s">
         <v>323</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>343</v>
+      </c>
+      <c r="C53" t="s">
+        <v>344</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3897,7 +3947,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Take out agent option for coordinator
</commit_message>
<xml_diff>
--- a/app/config/tables/business/forms/enrollment/enrollment.xlsx
+++ b/app/config/tables/business/forms/enrollment/enrollment.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\eKichabi\app-designer\app\config\tables\business\forms\enrollment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="40" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="5655" yWindow="45" windowWidth="25365" windowHeight="15825" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1104,7 +1109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2247,32 +2252,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="44.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
+    <col min="7" max="8" width="44.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.1640625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="16" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="2" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="22" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" style="1" customWidth="1"/>
-    <col min="19" max="1025" width="11.33203125" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="1"/>
+    <col min="18" max="18" width="17.140625" style="1" customWidth="1"/>
+    <col min="19" max="1025" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2333,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>160</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>98</v>
@@ -2363,7 +2368,7 @@
       <c r="H3" s="6"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:18" ht="120">
+    <row r="4" spans="1:18" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="D4" s="1" t="s">
         <v>237</v>
@@ -2376,7 +2381,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>12</v>
       </c>
@@ -2397,7 +2402,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>12</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>12</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>12</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>12</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="60">
+    <row r="11" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>12</v>
       </c>
@@ -2526,7 +2531,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>161</v>
       </c>
@@ -2549,7 +2554,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="60">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
         <v>161</v>
       </c>
@@ -2578,7 +2583,7 @@
       <c r="P13" s="23"/>
       <c r="Q13" s="23"/>
     </row>
-    <row r="14" spans="1:18" s="9" customFormat="1">
+    <row r="14" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="9" t="s">
         <v>98</v>
@@ -2591,7 +2596,7 @@
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
     </row>
-    <row r="15" spans="1:18" s="9" customFormat="1" ht="216">
+    <row r="15" spans="1:18" s="9" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>161</v>
       </c>
@@ -2623,7 +2628,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="9" customFormat="1">
+    <row r="16" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="9" t="s">
         <v>98</v>
@@ -2637,7 +2642,7 @@
       <c r="P16" s="25"/>
       <c r="Q16" s="28"/>
     </row>
-    <row r="17" spans="1:18" s="9" customFormat="1" ht="84">
+    <row r="17" spans="1:18" s="9" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A17" s="29"/>
       <c r="D17" s="9" t="s">
         <v>23</v>
@@ -2658,7 +2663,7 @@
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
-    <row r="18" spans="1:18" s="9" customFormat="1">
+    <row r="18" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29"/>
       <c r="B18" s="9" t="s">
         <v>135</v>
@@ -2668,7 +2673,7 @@
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
     </row>
-    <row r="19" spans="1:18" s="9" customFormat="1">
+    <row r="19" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="29"/>
       <c r="B19" s="9" t="s">
         <v>135</v>
@@ -2678,7 +2683,7 @@
       <c r="P19" s="25"/>
       <c r="Q19" s="25"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="13">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
         <v>12</v>
       </c>
@@ -2701,7 +2706,7 @@
       <c r="P20" s="23"/>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
         <v>12</v>
       </c>
@@ -2721,14 +2726,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="14" t="s">
         <v>205</v>
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:18" ht="101" customHeight="1">
+    <row r="23" spans="1:18" ht="101.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
         <v>164</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="84">
+    <row r="24" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="D24" s="1" t="s">
         <v>191</v>
@@ -2775,14 +2780,14 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="1" t="s">
         <v>206</v>
       </c>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:18" ht="24">
+    <row r="26" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
         <v>162</v>
       </c>
@@ -2805,7 +2810,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="48">
+    <row r="27" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
         <v>163</v>
       </c>
@@ -2834,7 +2839,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="1" t="s">
         <v>205</v>
@@ -2844,7 +2849,7 @@
       <c r="N28" s="23"/>
       <c r="Q28" s="26"/>
     </row>
-    <row r="29" spans="1:18" s="10" customFormat="1" ht="60">
+    <row r="29" spans="1:18" s="10" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
         <v>208</v>
       </c>
@@ -2876,7 +2881,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
         <v>166</v>
       </c>
@@ -2899,7 +2904,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
       <c r="B31" s="1" t="s">
         <v>206</v>
@@ -2907,7 +2912,7 @@
       <c r="H31" s="6"/>
       <c r="N31" s="23"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="29"/>
       <c r="B32" s="1" t="s">
         <v>205</v>
@@ -2915,7 +2920,7 @@
       <c r="H32" s="6"/>
       <c r="N32" s="23"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
       <c r="D33" s="1" t="s">
         <v>13</v>
@@ -2936,7 +2941,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="1" t="s">
         <v>211</v>
@@ -2947,7 +2952,7 @@
       <c r="H34" s="6"/>
       <c r="N34" s="23"/>
     </row>
-    <row r="35" spans="1:18" s="10" customFormat="1" ht="96">
+    <row r="35" spans="1:18" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
         <v>165</v>
       </c>
@@ -2979,7 +2984,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="48">
+    <row r="36" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A36" s="29" t="s">
         <v>166</v>
       </c>
@@ -3002,27 +3007,27 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="29"/>
       <c r="B37" s="1" t="s">
         <v>135</v>
       </c>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="29"/>
       <c r="B38" s="1" t="s">
         <v>206</v>
       </c>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
       <c r="B39" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="29"/>
       <c r="D40" s="1" t="s">
         <v>194</v>
@@ -3037,7 +3042,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="1" t="s">
         <v>135</v>
@@ -3062,22 +3067,22 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="15.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="33" style="1" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="32.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -3112,7 +3117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>239</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>79</v>
       </c>
@@ -3170,7 +3175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>187</v>
       </c>
@@ -3199,7 +3204,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1">
+    <row r="5" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -3228,12 +3233,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" customHeight="1">
+    <row r="6" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="8" spans="1:11" ht="85" customHeight="1">
+    <row r="8" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>134</v>
       </c>
@@ -3266,17 +3271,17 @@
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="1" customWidth="1"/>
-    <col min="5" max="1024" width="8.6640625" style="1" customWidth="1"/>
-    <col min="1025" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
+    <col min="5" max="1024" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1025" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.25" customHeight="1">
+    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -3304,7 +3309,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1">
+    <row r="3" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -3318,7 +3323,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" customHeight="1">
+    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -3346,7 +3351,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -3360,7 +3365,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -3374,7 +3379,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -3388,7 +3393,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>313</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>313</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>313</v>
       </c>
@@ -3444,7 +3449,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>232</v>
       </c>
@@ -3458,7 +3463,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>232</v>
       </c>
@@ -3472,7 +3477,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>232</v>
       </c>
@@ -3486,7 +3491,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>153</v>
       </c>
@@ -3500,7 +3505,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>153</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>59</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
@@ -3542,7 +3547,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>59</v>
       </c>
@@ -3556,7 +3561,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -3570,7 +3575,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -3598,7 +3603,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>113</v>
       </c>
@@ -3612,7 +3617,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>113</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>113</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>113</v>
       </c>
@@ -3668,7 +3673,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>113</v>
       </c>
@@ -3682,7 +3687,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -3710,7 +3715,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3724,7 +3729,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3738,7 +3743,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -3752,7 +3757,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3780,7 +3785,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -3794,7 +3799,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>113</v>
       </c>
@@ -3808,7 +3813,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
@@ -3836,7 +3841,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -3864,7 +3869,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>113</v>
       </c>
@@ -3878,7 +3883,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>113</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>113</v>
       </c>
@@ -3906,7 +3911,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
@@ -3920,7 +3925,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
@@ -3934,25 +3939,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -3977,18 +3982,18 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" style="1" customWidth="1"/>
-    <col min="7" max="1022" width="11.33203125" style="1" customWidth="1"/>
-    <col min="1023" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="28.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="1022" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1023" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.75" customHeight="1">
+    <row r="1" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -4008,7 +4013,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.75" customHeight="1">
+    <row r="2" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -4016,7 +4021,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.75" customHeight="1">
+    <row r="3" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -4024,7 +4029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.75" customHeight="1">
+    <row r="4" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -4032,7 +4037,7 @@
         <v>20180703</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.75" customHeight="1">
+    <row r="5" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -4043,7 +4048,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4051,7 +4056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -4062,7 +4067,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>169</v>
       </c>
@@ -4088,23 +4093,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.1640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="20.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
@@ -4112,7 +4117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4122,27 +4127,27 @@
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -4150,7 +4155,7 @@
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4160,7 +4165,7 @@
       <c r="C6"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4171,7 +4176,7 @@
       <c r="D7"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -4182,7 +4187,7 @@
       <c r="D8"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -4194,7 +4199,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" s="14" customFormat="1">
+    <row r="10" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>201</v>
       </c>
@@ -4204,7 +4209,7 @@
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" s="14" customFormat="1">
+    <row r="11" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
@@ -4212,7 +4217,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1">
+    <row r="12" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>23</v>
       </c>
@@ -4222,7 +4227,7 @@
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:8" s="14" customFormat="1">
+    <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>35</v>
       </c>
@@ -4232,7 +4237,7 @@
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:8" s="14" customFormat="1">
+    <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>191</v>
       </c>
@@ -4240,7 +4245,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1">
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
@@ -4250,7 +4255,7 @@
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:8" s="14" customFormat="1">
+    <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
@@ -4260,7 +4265,7 @@
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" s="14" customFormat="1">
+    <row r="17" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -4270,7 +4275,7 @@
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" s="14" customFormat="1">
+    <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>174</v>
       </c>
@@ -4280,7 +4285,7 @@
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" s="14" customFormat="1">
+    <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>13</v>
       </c>
@@ -4288,7 +4293,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="14" customFormat="1">
+    <row r="20" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>23</v>
       </c>
@@ -4298,7 +4303,7 @@
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" s="14" customFormat="1">
+    <row r="21" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>174</v>
       </c>
@@ -4308,7 +4313,7 @@
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -4316,7 +4321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -4324,7 +4329,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -4332,7 +4337,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -4340,7 +4345,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -4348,7 +4353,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -4356,7 +4361,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>217</v>
       </c>
@@ -4364,7 +4369,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>217</v>
       </c>
@@ -4372,7 +4377,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>217</v>
       </c>
@@ -4380,7 +4385,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -4388,7 +4393,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -4396,7 +4401,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4423,14 +4428,14 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -4438,7 +4443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>221</v>
       </c>
@@ -4446,7 +4451,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="14"/>
     </row>
   </sheetData>
@@ -4467,13 +4472,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>212</v>
       </c>
@@ -4481,7 +4486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="211" customHeight="1">
+    <row r="2" spans="1:2" ht="210.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -4489,7 +4494,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="174" customHeight="1">
+    <row r="3" spans="1:2" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -4497,7 +4502,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="175" customHeight="1">
+    <row r="4" spans="1:2" ht="174.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>245</v>
       </c>
@@ -4505,7 +4510,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
     </row>
   </sheetData>

</xml_diff>